<commit_message>
TP#20088: Update Canada Freight to account for the correct amount of packages
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/CA Freight Dom.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/CA Freight Dom.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="127">
   <si>
     <t>RTC</t>
   </si>
@@ -332,10 +332,6 @@
   </si>
   <si>
     <t>ProcessShipmentRequest.RequestedShipment.Recipient.Address</t>
-  </si>
-  <si>
-    <t>CA Freight
- Domestic</t>
   </si>
   <si>
     <t>ProcessShipmentRequest.RequestedShipment.ShippingChargesPayment.Payor.ResponsibleParty</t>
@@ -2038,7 +2034,7 @@
   <dimension ref="A1:ED8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2160,22 +2156,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:134" s="6" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="22"/>
+      <c r="A1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
+        <v>58</v>
+      </c>
       <c r="D1" s="23" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>22</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>34</v>
@@ -2186,14 +2184,14 @@
       <c r="J1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>34</v>
+      <c r="K1" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="11" t="s">
-        <v>94</v>
+      <c r="M1" s="24" t="s">
+        <v>60</v>
       </c>
       <c r="N1" s="24" t="s">
         <v>60</v>
@@ -2202,7 +2200,7 @@
         <v>60</v>
       </c>
       <c r="P1" s="24" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="Q1" s="24" t="s">
         <v>101</v>
@@ -2220,7 +2218,7 @@
         <v>101</v>
       </c>
       <c r="V1" s="24" t="s">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="W1" s="24" t="s">
         <v>36</v>
@@ -2229,7 +2227,7 @@
         <v>36</v>
       </c>
       <c r="Y1" s="24" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="Z1" s="24" t="s">
         <v>102</v>
@@ -2246,29 +2244,29 @@
       <c r="AD1" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="AE1" s="24" t="s">
-        <v>102</v>
+      <c r="AE1" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="AG1" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AH1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AI1" s="4" t="s">
-        <v>105</v>
+      <c r="AI1" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="AJ1" s="24" t="s">
         <v>109</v>
       </c>
       <c r="AK1" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AL1" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM1" s="24" t="s">
         <v>110</v>
@@ -2280,22 +2278,22 @@
         <v>112</v>
       </c>
       <c r="AP1" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="AQ1" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR1" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="AS1" s="24" t="s">
         <v>113</v>
-      </c>
-      <c r="AQ1" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="AR1" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS1" s="24" t="s">
-        <v>109</v>
       </c>
       <c r="AT1" s="24" t="s">
         <v>114</v>
       </c>
       <c r="AU1" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AV1" s="24" t="s">
         <v>115</v>
@@ -2304,104 +2302,102 @@
         <v>116</v>
       </c>
       <c r="AX1" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AY1" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="AZ1" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="AY1" s="24" t="s">
+      <c r="BA1" s="24" t="s">
         <v>117</v>
-      </c>
-      <c r="AZ1" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA1" s="24" t="s">
-        <v>118</v>
       </c>
       <c r="BB1" s="24" t="s">
         <v>118</v>
       </c>
       <c r="BC1" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="BD1" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="BE1" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="BF1" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="BG1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="BD1" s="24" t="s">
+      <c r="BH1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="BE1" s="24" t="s">
+      <c r="BI1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="BF1" s="24" t="s">
+      <c r="BJ1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="BG1" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="BH1" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="BI1" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="BJ1" s="24" t="s">
-        <v>120</v>
-      </c>
       <c r="BK1" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="BL1" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="BM1" s="24" t="s">
         <v>120</v>
       </c>
       <c r="BN1" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="BO1" s="24" t="s">
         <v>121</v>
       </c>
       <c r="BP1" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="BQ1" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="BR1" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="BS1" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="BT1" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="BU1" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="BV1" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="BW1" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="BQ1" s="24" t="s">
+      <c r="BX1" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="BR1" s="24" t="s">
+      <c r="BY1" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="BS1" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="BT1" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="BU1" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="BV1" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="BW1" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="BX1" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="BY1" s="25" t="s">
-        <v>123</v>
-      </c>
       <c r="BZ1" s="24" t="s">
-        <v>123</v>
+        <v>34</v>
       </c>
       <c r="CA1" s="24" t="s">
         <v>34</v>
       </c>
       <c r="CB1" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="CC1" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="CD1" s="26" t="s">
-        <v>106</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="CC1" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="CJ1" s="12"/>
       <c r="CK1" s="12"/>
       <c r="CL1" s="12"/>
       <c r="CM1" s="12"/>
@@ -2419,420 +2415,418 @@
       <c r="CY1" s="12"/>
       <c r="CZ1" s="12"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="12"/>
     </row>
     <row r="2" spans="1:134" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>59</v>
       </c>
+      <c r="D2" s="31"/>
       <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="F2" s="31" t="s">
+        <v>23</v>
+      </c>
       <c r="G2" s="31" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K2" s="31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="X2" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y2" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z2" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA2" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB2" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF2" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG2" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH2" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI2" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ2" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK2" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL2" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM2" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN2" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="AO2" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP2" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ2" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR2" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS2" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT2" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU2" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV2" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW2" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX2" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="AY2" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="BA2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="S2" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="U2" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="X2" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y2" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z2" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA2" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB2" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC2" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD2" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE2" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF2" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG2" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH2" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI2" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ2" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK2" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL2" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="AM2" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN2" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO2" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="AP2" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="AQ2" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR2" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS2" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="AT2" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="AU2" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV2" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="AW2" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="AX2" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="AY2" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="AZ2" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA2" s="31" t="s">
+      <c r="BB2" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="BC2" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="BD2" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="BE2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="BB2" s="31" t="s">
+      <c r="BF2" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG2" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH2" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="BI2" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="BJ2" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="BK2" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL2" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="BM2" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="BN2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="BC2" s="31" t="s">
+      <c r="BO2" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="BD2" s="31" t="s">
+      <c r="BP2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="BE2" s="31" t="s">
+      <c r="BQ2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="BF2" s="31" t="s">
+      <c r="BR2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="BG2" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="BH2" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="BI2" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="BJ2" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="BK2" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="BL2" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="BM2" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="BN2" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="BO2" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="BP2" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="BQ2" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="BR2" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="BS2" s="31" t="s">
-        <v>43</v>
+      <c r="BS2" s="32" t="s">
+        <v>6</v>
       </c>
       <c r="BT2" s="32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BU2" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="BV2" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="BW2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="BV2" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="BW2" s="32" t="s">
-        <v>87</v>
-      </c>
       <c r="BX2" s="32" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="BY2" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="BZ2" s="32" t="s">
         <v>92</v>
       </c>
+      <c r="BZ2" s="31" t="s">
+        <v>9</v>
+      </c>
       <c r="CA2" s="31" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="CB2" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="CC2" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="CD2" s="33" t="s">
+      <c r="CC2" s="33" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:134" s="14" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="20" t="b">
+      <c r="A3" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="E3" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="28">
+        <v>20000</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="W3" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="X3" s="28">
+        <v>1234567890</v>
+      </c>
+      <c r="Y3" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z3" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB3" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC3" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF3" s="28">
+        <v>150067600</v>
+      </c>
+      <c r="AG3" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH3" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI3" s="28">
+        <v>602091147</v>
+      </c>
+      <c r="AJ3" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK3" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL3" s="28">
+        <v>5166829292</v>
+      </c>
+      <c r="AM3" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN3" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP3" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ3" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR3" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS3" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT3" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU3" s="28">
+        <v>200</v>
+      </c>
+      <c r="AV3" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW3" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX3" s="28">
+        <v>50</v>
+      </c>
+      <c r="AY3" s="28">
+        <v>1</v>
+      </c>
+      <c r="AZ3" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="BA3" s="28">
+        <v>50</v>
+      </c>
+      <c r="BB3" s="28">
+        <v>180</v>
+      </c>
+      <c r="BC3" s="28">
         <v>93</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="28">
-        <v>20000</v>
-      </c>
-      <c r="N3" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="P3" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="R3" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="T3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="U3" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28" t="s">
+      <c r="BD3" s="28">
+        <v>106</v>
+      </c>
+      <c r="BE3" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="BF3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="BG3" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BH3" s="28">
         <v>1</v>
-      </c>
-      <c r="X3" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y3" s="28">
-        <v>1234567890</v>
-      </c>
-      <c r="Z3" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA3" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB3" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC3" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD3" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="AG3" s="28">
-        <v>150067600</v>
-      </c>
-      <c r="AH3" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI3" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ3" s="28">
-        <v>602091147</v>
-      </c>
-      <c r="AK3" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="AL3" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM3" s="28">
-        <v>5166829292</v>
-      </c>
-      <c r="AN3" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="AO3" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="AP3" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ3" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="AR3" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="AS3" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT3" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="AU3" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV3" s="28">
-        <v>200</v>
-      </c>
-      <c r="AW3" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="AX3" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="AY3" s="28">
-        <v>50</v>
-      </c>
-      <c r="AZ3" s="28">
-        <v>1</v>
-      </c>
-      <c r="BA3" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="BB3" s="28">
-        <v>50</v>
-      </c>
-      <c r="BC3" s="28">
-        <v>180</v>
-      </c>
-      <c r="BD3" s="28">
-        <v>93</v>
-      </c>
-      <c r="BE3" s="28">
-        <v>106</v>
-      </c>
-      <c r="BF3" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="BG3" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="BH3" s="28" t="s">
-        <v>82</v>
       </c>
       <c r="BI3" s="28">
         <v>1</v>
@@ -2840,66 +2834,64 @@
       <c r="BJ3" s="28">
         <v>1</v>
       </c>
-      <c r="BK3" s="28">
+      <c r="BK3" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="BL3" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="BM3" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="BN3" s="28">
+        <v>50</v>
+      </c>
+      <c r="BO3" s="28">
+        <v>180</v>
+      </c>
+      <c r="BP3" s="28">
+        <v>93</v>
+      </c>
+      <c r="BQ3" s="28">
+        <v>106</v>
+      </c>
+      <c r="BR3" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="BS3" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="BT3" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="BU3" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV3" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="BW3" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="BX3" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="BY3" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="BL3" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="BM3" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="BN3" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="BO3" s="28">
-        <v>50</v>
-      </c>
-      <c r="BP3" s="28">
-        <v>180</v>
-      </c>
-      <c r="BQ3" s="28">
-        <v>93</v>
-      </c>
-      <c r="BR3" s="28">
-        <v>106</v>
-      </c>
-      <c r="BS3" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="BT3" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="BU3" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="BV3" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="BW3" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="BX3" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="BY3" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="BZ3" s="28" t="b">
+      <c r="BZ3" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="CA3" s="28">
         <v>1</v>
       </c>
-      <c r="CA3" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="CB3" s="28">
-        <v>1</v>
-      </c>
-      <c r="CC3" s="28" t="s">
+      <c r="CB3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="CD3" s="29" t="s">
+      <c r="CC3" s="29" t="s">
         <v>11</v>
       </c>
+      <c r="CJ3" s="15"/>
       <c r="CK3" s="15"/>
       <c r="CL3" s="15"/>
       <c r="CM3" s="15"/>
@@ -2917,15 +2909,15 @@
       <c r="CY3" s="15"/>
       <c r="CZ3" s="15"/>
       <c r="DA3" s="15"/>
-      <c r="DB3" s="15"/>
-      <c r="DC3" s="16"/>
+      <c r="DB3" s="16"/>
+      <c r="DC3" s="17"/>
       <c r="DD3" s="17"/>
       <c r="DE3" s="17"/>
       <c r="DF3" s="17"/>
       <c r="DG3" s="17"/>
       <c r="DH3" s="17"/>
       <c r="DI3" s="17"/>
-      <c r="DJ3" s="17"/>
+      <c r="DJ3" s="16"/>
       <c r="DK3" s="16"/>
       <c r="DL3" s="16"/>
       <c r="DM3" s="16"/>
@@ -2945,7 +2937,6 @@
       <c r="EA3" s="16"/>
       <c r="EB3" s="16"/>
       <c r="EC3" s="16"/>
-      <c r="ED3" s="16"/>
     </row>
     <row r="4" spans="1:134" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>

</xml_diff>